<commit_message>
[Document, Modified]: TaskList(2) and Login-Logout Specification
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/UseCase/TaskList/TaskList(2) Specification.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/UseCase/TaskList/TaskList(2) Specification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Search information" sheetId="1" state="visible" r:id="rId2"/>
@@ -47,390 +47,167 @@
     <t xml:space="preserve">Actor(s):</t>
   </si>
   <si>
+    <t xml:space="preserve">User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summary:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giúp người dùng có thể tìm kiếm thông tin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basle course of events:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actor actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System response</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Người dùng nhập thông tin cần tìm kiếm
+- Hệ thống sẽ ghi nhận thông tin mà người dùng nhập vào
+- Người dùng nhấp chọn "Search"
+- Hệ thống sẽ tìm kiếm và trả về thông tin mà người dùng đã nhập</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Người dùng nhập thông tin cần tìm kiếm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Hệ thống sẽ ghi nhận thông tin mà người dùng nhập vào</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Người dùng nhấp chọn "Search"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Hệ thống sẽ tìm kiếm và trả về thông tin mà người dùng đã nhập</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alternative paths:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Không có</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exception paths:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lỗi mã nguồn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension points:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Người dùng nhập thông tin vào ô tìm kiếm ở menu chính của phần mềm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triggers:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Người dùng nhấp vào "Search"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre-condition:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ô tìm kiếm phải có thông tin được nhập vào từ người dùng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Post-condition:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hệ thống trả về thông tin mà người dùng tìm kiếm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giúp người dùng có thể sắp xếp thông tin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Người dùng nhấp chọn "Sort"
+- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc sắp xếp
+- Người dùng nhấp chọn tiêu chí cần sắp xếp
+- Hệ thống sẽ sắp xếp các thông tin dựa trên tiêu chí mà người dùng đã chọn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Người dùng nhấp chọn "Sort"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc sắp xếp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Người dùng nhấp chọn tiêu chí cần sắp xếp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Hệ thống sẽ sắp xếp các thông tin dựa trên tiêu chí mà người dùng đã chọn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Có bug trong phần mềm cản trở việc sắp xếp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Người dùng nhấp chọn "Sort" ở menu chính của phần mềm bên phải ô tìm kiếm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Người dùng nhấp chọn tiêu chí cần sắp xếp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phải có thông tin trong phần mềm để có thể sắp xếp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hệ thống trả về thông tin mà người dùng sắp xếp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort by name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giúp người dùng có thể sắp xếp thông tin theo phạm vi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Người dùng nhấp chọn "Sort"
+- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc sắp xếp
+- Người dùng nhấp chọn "sort by name"
+- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc sắp xếp cho sort by name
+- Người dùng nhấp chọn tiêu chí cần sắp xếp
+- Hệ thống sẽ sắp xếp các thông tin dựa trên tiêu chí mà người dùng đã chọn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Người dùng nhấp chọn "sort by name"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc sắp xếp cho sort by name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort by date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giúp người dùng có thể sắp xếp thông tin theo ngày</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Người dùng nhấp chọn "Sort"
+- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc sắp xếp
+- Người dùng nhấp chọn "sort by date"
+- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc sắp xếp
+- Người dùng nhấp chọn tiêu chí cần sắp xếp
+- Hệ thống sẽ sắp xếp các thông tin dựa trên tiêu chí mà người dùng đã chọn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Người dùng nhấp chọn "sort by date"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group by</t>
+  </si>
+  <si>
     <t xml:space="preserve">User, Admin</t>
   </si>
   <si>
-    <t xml:space="preserve">Summary:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Giúp người dùng có thể tìm kiếm thông tin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basle course of events:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actor actions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">System response</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhập thông tin cần tìm kiếm
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ ghi nhận thông tin mà người dùng nhập vào
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "Search"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ tìm kiếm và trả về thông tin mà người dùng đã nhập</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">- Người dùng nhập thông tin cần tìm kiếm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Hệ thống sẽ ghi nhận thông tin mà người dùng nhập vào</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Người dùng nhấp chọn "Search"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Hệ thống sẽ tìm kiếm và trả về thông tin mà người dùng đã nhập</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alternative paths:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Không có</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exception paths:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lỗi mã nguồn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension points:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Người dùng nhập thông tin vào ô tìm kiếm ở menu chính của phần mềm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Triggers:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Người dùng nhấp vào "Search"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre-condition:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ô tìm kiếm phải có thông tin được nhập vào từ người dùng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Post-condition:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hệ thống trả về thông tin mà người dùng tìm kiếm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sort by</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Giúp người dùng có thể sắp xếp thông tin</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "Sort"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc sắp xếp
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn tiêu chí cần sắp xếp
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ sắp xếp các thông tin dựa trên tiêu chí mà người dùng đã chọn</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">- Người dùng nhấp chọn "Sort"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc sắp xếp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Người dùng nhấp chọn tiêu chí cần sắp xếp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Hệ thống sẽ sắp xếp các thông tin dựa trên tiêu chí mà người dùng đã chọn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Có bug trong phần mềm cản trở việc sắp xếp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Người dùng nhấp chọn "Sort" ở menu chính của phần mềm bên phải ô tìm kiếm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Người dùng nhấp chọn tiêu chí cần sắp xếp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phải có thông tin trong phần mềm để có thể sắp xếp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hệ thống trả về thông tin mà người dùng sắp xếp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sort by name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Giúp người dùng có thể sắp xếp thông tin theo phạm vi</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "Sort"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc sắp xếp
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "sort by name"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc sắp xếp cho sort by name
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn tiêu chí cần sắp xếp
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ sắp xếp các thông tin dựa trên tiêu chí mà người dùng đã chọn</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">- Người dùng nhấp chọn "sort by name"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc sắp xếp cho sort by name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sort by date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Giúp người dùng có thể sắp xếp thông tin theo ngày</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "Sort"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc sắp xếp
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "sort by date"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc sắp xếp
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn tiêu chí cần sắp xếp
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ sắp xếp các thông tin dựa trên tiêu chí mà người dùng đã chọn</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">- Người dùng nhấp chọn "sort by date"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group by</t>
-  </si>
-  <si>
     <t xml:space="preserve">Giúp người dùng có thể gom nhóm thông tin</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "Group"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc gom nhóm
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn tiêu chí cần gom nhóm
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ gom nhóm các thông tin dựa trên tiêu chí mà người dùng đã chọn</t>
-    </r>
+    <t xml:space="preserve">- Người dùng nhấp chọn "Group"
+- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc gom nhóm
+- Người dùng nhấp chọn tiêu chí cần gom nhóm
+- Hệ thống sẽ gom nhóm các thông tin dựa trên tiêu chí mà người dùng đã chọn</t>
   </si>
   <si>
     <t xml:space="preserve">- Người dùng nhấp chọn "Group"</t>
@@ -463,47 +240,10 @@
     <t xml:space="preserve">Giúp người dùng có thể gom nhóm thông tin theo từng phần</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "Group"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc gom nhóm
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "group by section"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ gom nhóm các thông tin theo từng phần</t>
-    </r>
+    <t xml:space="preserve">- Người dùng nhấp chọn "Group"
+- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc gom nhóm
+- Người dùng nhấp chọn "group by section"
+- Hệ thống sẽ gom nhóm các thông tin theo từng phần</t>
   </si>
   <si>
     <t xml:space="preserve">- Người dùng nhấp chọn "group by section"</t>
@@ -527,47 +267,10 @@
     <t xml:space="preserve">Giúp người dùng có thể gom nhóm thông tin theo độ ưu tiên</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "Group"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc gom nhóm
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "group by priority"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ gom nhóm các thông tin theo độ ưu tiên</t>
-    </r>
+    <t xml:space="preserve">- Người dùng nhấp chọn "Group"
+- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc gom nhóm
+- Người dùng nhấp chọn "group by priority"
+- Hệ thống sẽ gom nhóm các thông tin theo độ ưu tiên</t>
   </si>
   <si>
     <t xml:space="preserve">- Người dùng nhấp chọn "group by priority"</t>
@@ -591,47 +294,10 @@
     <t xml:space="preserve">Giúp người dùng có thể gom nhóm thông tin theo tiến độ công việc</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "Group"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc gom nhóm
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "group by progress"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ gom nhóm các thông tin theo tiến độ công việc</t>
-    </r>
+    <t xml:space="preserve">- Người dùng nhấp chọn "Group"
+- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc gom nhóm
+- Người dùng nhấp chọn "group by progress"
+- Hệ thống sẽ gom nhóm các thông tin theo tiến độ công việc</t>
   </si>
   <si>
     <t xml:space="preserve">- Người dùng nhấp chọn "group by progress"</t>
@@ -655,47 +321,10 @@
     <t xml:space="preserve">Giúp người dùng có thể gom nhóm thông tin theo loại công việc</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "Group"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc gom nhóm
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "group by tag"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ gom nhóm các thông tin theo loại công việc</t>
-    </r>
+    <t xml:space="preserve">- Người dùng nhấp chọn "Group"
+- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc gom nhóm
+- Người dùng nhấp chọn "group by tag"
+- Hệ thống sẽ gom nhóm các thông tin theo loại công việc</t>
   </si>
   <si>
     <t xml:space="preserve">- Người dùng nhấp chọn "group by tag"</t>
@@ -719,84 +348,18 @@
     <t xml:space="preserve">Giúp người dùng có thể gom nhóm thông tin theo ngày hết hạn công việc</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "Group by"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc gom nhóm</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 
+    <t xml:space="preserve">- Người dùng nhấp chọn "Group by"
+- Hệ thống sẽ hiển thị danh mục các tiêu chí cho việc gom nhóm 
 - Người dùng nhấp chọn "group by end date"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tùy chọn cho "group by end date" bao gồm: "before deadline", "deadline",  "out of deadline"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">*
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "before deadline"
+- Hệ thống sẽ hiển thị danh mục các tùy chọn cho "group by end date" bao gồm: "before deadline", "deadline",  "out of deadline"
+*
+- Người dùng nhấp chọn "before deadline"
 - Hệ thống sẽ gom nhóm các task trước ngày hết hạn cho người dùng
 - Người dùng nhấp chọn "deadline"
 - Hệ thống sẽ gom nhóm các task đúng ngày hết hạn cho người dùng
 - Người dùng nhấp chọn "out of deadline"
 - Hệ thống sẽ gom nhóm các task trễ deadline cho người dùng
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">*</t>
-    </r>
+*</t>
   </si>
   <si>
     <t xml:space="preserve">- Người dùng nhấp chọn "Group by"</t>
@@ -847,80 +410,14 @@
     <t xml:space="preserve">Giúp người dùng có thể lọc theo biểu thức chính quy</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "icon menu"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tùy chọn
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "filter query"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị 1 ô text để người dùng nhập biểu thức chính quy
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhập biểu thức chính quy
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ ghi nhận biểu thức chính quy do người dùng nhập vào
+    <t xml:space="preserve">- Người dùng nhấp chọn "icon menu"
+- Hệ thống sẽ hiển thị danh mục các tùy chọn
+- Người dùng nhấp chọn "filter query"
+- Hệ thống sẽ hiển thị 1 ô text để người dùng nhập biểu thức chính quy
+- Người dùng nhập biểu thức chính quy
+- Hệ thống sẽ ghi nhận biểu thức chính quy do người dùng nhập vào
 - Người dùng nhấp "Enter" từ bàn phím
-- Hệ thống sẽ lọc thông tin theo biểu thức chính quy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+- Hệ thống sẽ lọc thông tin theo biểu thức chính quy </t>
   </si>
   <si>
     <t xml:space="preserve">- Người dùng nhấp chọn "icon menu"</t>
@@ -965,68 +462,12 @@
     <t xml:space="preserve">Giúp người dùng có thể điều chỉnh giao diện</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "Setting"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tùy chọn
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "set layout"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị thêm 2 mục nhỏ chứa các chế độ layout
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn chế độ layout
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ thay đổi layout cho phần mềm</t>
-    </r>
+    <t xml:space="preserve">- Người dùng nhấp chọn "Setting"
+- Hệ thống sẽ hiển thị danh mục các tùy chọn
+- Người dùng nhấp chọn "set layout"
+- Hệ thống sẽ hiển thị thêm 2 mục nhỏ chứa các chế độ layout
+- Người dùng nhấp chọn chế độ layout
+- Hệ thống sẽ thay đổi layout cho phần mềm</t>
   </si>
   <si>
     <t xml:space="preserve">- Người dùng nhấp chọn "Setting"</t>
@@ -1059,68 +500,12 @@
     <t xml:space="preserve">Giúp người dùng có thể thay đổi giao diện phần mềm sang dạng bảng</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "Setting"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị danh mục các tùy chọn
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "set layout"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ hiển thị thêm 2 mục nhỏ chứa các chế độ layout
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">- Người dùng nhấp chọn "set layout board"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">- Hệ thống sẽ thay đổi giao diện phần mềm sang dạng bảng</t>
-    </r>
+    <t xml:space="preserve">- Người dùng nhấp chọn "Setting"
+- Hệ thống sẽ hiển thị danh mục các tùy chọn
+- Người dùng nhấp chọn "set layout"
+- Hệ thống sẽ hiển thị thêm 2 mục nhỏ chứa các chế độ layout
+- Người dùng nhấp chọn "set layout board"
+- Hệ thống sẽ thay đổi giao diện phần mềm sang dạng bảng</t>
   </si>
   <si>
     <t xml:space="preserve">- Người dùng nhấp chọn "set layout board"</t>
@@ -1157,7 +542,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1196,12 +581,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1215,12 +594,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1272,7 +645,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1285,24 +658,20 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1324,11 +693,11 @@
   </sheetPr>
   <dimension ref="B2:D14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.7"/>
@@ -1519,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -1709,7 +1078,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -1755,10 +1124,10 @@
     </row>
     <row r="9" customFormat="false" ht="71.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="5"/>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1890,7 +1259,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -2028,7 +1397,7 @@
   </sheetPr>
   <dimension ref="B2:D15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2062,7 +1431,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -2234,7 +1603,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -2406,7 +1775,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -2415,7 +1784,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -2432,22 +1801,22 @@
     </row>
     <row r="7" customFormat="false" ht="92.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="92.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2464,7 +1833,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="5"/>
     </row>
@@ -2473,7 +1842,7 @@
         <v>19</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="5"/>
     </row>
@@ -2482,7 +1851,7 @@
         <v>21</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="5"/>
     </row>
@@ -2491,7 +1860,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="5"/>
     </row>
@@ -2500,7 +1869,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="5"/>
     </row>
@@ -2560,7 +1929,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="5"/>
     </row>
@@ -2569,7 +1938,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -2578,7 +1947,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -2595,31 +1964,31 @@
     </row>
     <row r="7" customFormat="false" ht="86.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="86.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="86.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2645,7 +2014,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="5"/>
     </row>
@@ -2654,7 +2023,7 @@
         <v>21</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="5"/>
     </row>
@@ -2663,7 +2032,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="5"/>
     </row>
@@ -2672,7 +2041,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="5"/>
     </row>
@@ -2732,7 +2101,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="5"/>
     </row>
@@ -2741,7 +2110,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -2750,7 +2119,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -2767,31 +2136,31 @@
     </row>
     <row r="7" customFormat="false" ht="86.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="86.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="86.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2817,7 +2186,7 @@
         <v>19</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="5"/>
     </row>
@@ -2826,7 +2195,7 @@
         <v>21</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="5"/>
     </row>
@@ -2835,7 +2204,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="5"/>
     </row>
@@ -2844,7 +2213,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="5"/>
     </row>
@@ -2904,7 +2273,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="5"/>
     </row>
@@ -2913,7 +2282,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -3076,7 +2445,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -3239,7 +2608,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -3402,7 +2771,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5"/>
     </row>
@@ -3568,7 +2937,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5"/>
     </row>

</xml_diff>